<commit_message>
Updated CSV and Excel Workbook
</commit_message>
<xml_diff>
--- a/EndDeviceRelease.xlsx
+++ b/EndDeviceRelease.xlsx
@@ -9,26 +9,28 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="EndDeviceRecord" sheetId="1" r:id="rId1"/>
+    <sheet name="EndDeviceReleaseDetails" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="45">
   <si>
     <t>Device EUI</t>
   </si>
   <si>
+    <t>Hardware Revision</t>
+  </si>
+  <si>
+    <t>Install Code</t>
+  </si>
+  <si>
     <t>Datalogger Firmware Revision</t>
   </si>
   <si>
@@ -38,23 +40,128 @@
     <t>Router Firmware Revision</t>
   </si>
   <si>
+    <t>Meter EndPoint</t>
+  </si>
+  <si>
+    <t>0x541DFB00000006E0</t>
+  </si>
+  <si>
+    <t>0x541DFB00000006E1</t>
+  </si>
+  <si>
+    <t>0x541DFB00000006E2</t>
+  </si>
+  <si>
+    <t>20130826_1</t>
+  </si>
+  <si>
+    <t>0x541DFB00000006E3</t>
+  </si>
+  <si>
+    <t>0x541DFB00000006E4</t>
+  </si>
+  <si>
+    <t>0x541DFB00000006E5</t>
+  </si>
+  <si>
+    <t>0x541DFB00000006E6</t>
+  </si>
+  <si>
+    <t>0x541DFB00000006E7</t>
+  </si>
+  <si>
+    <t>0x541DFB00000006E8</t>
+  </si>
+  <si>
+    <t>0x541DFB00000006E9</t>
+  </si>
+  <si>
+    <t>20130826_2</t>
+  </si>
+  <si>
+    <t>0x541DFB00000006EA</t>
+  </si>
+  <si>
     <t>0x541DFB00000006EB</t>
   </si>
   <si>
-    <t>Device Type</t>
-  </si>
-  <si>
-    <t>ZGL</t>
-  </si>
-  <si>
-    <t>Install Code</t>
+    <t>20130827_1</t>
+  </si>
+  <si>
+    <t>0x000102030405060708090A0B0C0D0E0F</t>
+  </si>
+  <si>
+    <t>0x541DFB00000006EC</t>
+  </si>
+  <si>
+    <t>0x541DFB00000006ED</t>
+  </si>
+  <si>
+    <t>0x541DFB00000006EE</t>
+  </si>
+  <si>
+    <t>0x541DFB00000006EF</t>
+  </si>
+  <si>
+    <t>0x541DFB00000006F0</t>
+  </si>
+  <si>
+    <t>0x541DFB00000006F1</t>
+  </si>
+  <si>
+    <t>0x541DFB00000006F2</t>
+  </si>
+  <si>
+    <t>0x541DFB00000006F3</t>
+  </si>
+  <si>
+    <t>0x541DFB00000006F4</t>
+  </si>
+  <si>
+    <t>0x541DFB00000006F5</t>
+  </si>
+  <si>
+    <t>0x541DFB00000006F6</t>
+  </si>
+  <si>
+    <t>0x541DFB00000006F7</t>
+  </si>
+  <si>
+    <t>0x541DFB00000006F8</t>
+  </si>
+  <si>
+    <t>0x541DFB00000006F9</t>
+  </si>
+  <si>
+    <t>0x541DFB00000006FA</t>
+  </si>
+  <si>
+    <t>0x541DFB00000006FB</t>
+  </si>
+  <si>
+    <t>0x541DFB00000006FC</t>
+  </si>
+  <si>
+    <t>0x541DFB00000006FD</t>
+  </si>
+  <si>
+    <t>0x541DFB00000006FE</t>
+  </si>
+  <si>
+    <t>0x541DFB00000006FF</t>
+  </si>
+  <si>
+    <t>Release Number</t>
+  </si>
+  <si>
+    <t>Current Release Number</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -62,16 +169,316 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -79,15 +486,204 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="42">
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -365,51 +961,289 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:H33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9:B10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="19.85546875" customWidth="1"/>
-    <col min="4" max="4" width="28" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="C1" t="s">
+      <c r="H1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>7</v>
       </c>
-      <c r="D1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>6</v>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" t="s">
+        <v>21</v>
+      </c>
+      <c r="D13" t="s">
+        <v>22</v>
+      </c>
+      <c r="E13">
+        <v>1355</v>
+      </c>
+      <c r="F13">
+        <v>75</v>
+      </c>
+      <c r="H13">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" t="s">
+        <v>21</v>
+      </c>
+      <c r="D14" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>25</v>
+      </c>
+      <c r="B16" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B17" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>27</v>
+      </c>
+      <c r="B18" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
.xlsx file update with autopopulate data, .csv is a copy of this file
</commit_message>
<xml_diff>
--- a/EndDeviceRelease.xlsx
+++ b/EndDeviceRelease.xlsx
@@ -9,18 +9,18 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
   </bookViews>
   <sheets>
-    <sheet name="EndDeviceRecord" sheetId="1" r:id="rId1"/>
+    <sheet name="EndDeviceRelease" sheetId="1" r:id="rId1"/>
     <sheet name="EndDeviceReleaseDetails" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="48">
   <si>
     <t>Device EUI</t>
   </si>
@@ -155,6 +155,15 @@
   </si>
   <si>
     <t>Current Release Number</t>
+  </si>
+  <si>
+    <t>xx</t>
+  </si>
+  <si>
+    <t>yy</t>
+  </si>
+  <si>
+    <t>zz</t>
   </si>
 </sst>
 </file>
@@ -963,14 +972,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="36.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -1003,202 +1018,928 @@
       <c r="A2" t="s">
         <v>7</v>
       </c>
+      <c r="C2" t="e">
+        <f>VLOOKUP(B2,EndDeviceReleaseDetails!A$2:H$10000,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D2" t="e">
+        <f>VLOOKUP(B2,EndDeviceReleaseDetails!A$2:H$10000,3,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="E2" t="e">
+        <f>VLOOKUP(B2,EndDeviceReleaseDetails!A$2:H$10000,4,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="F2" t="e">
+        <f>VLOOKUP(B2,EndDeviceReleaseDetails!A$2:H$10000,5,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="G2" t="e">
+        <f>VLOOKUP(B2,EndDeviceReleaseDetails!A$2:H$10000,6,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="H2" t="e">
+        <f>VLOOKUP(B2,EndDeviceReleaseDetails!A$2:H$10000,7,FALSE)</f>
+        <v>#N/A</v>
+      </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
+      <c r="C3" t="e">
+        <f>VLOOKUP(B3,EndDeviceReleaseDetails!A$2:H$10000,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D3" t="e">
+        <f>VLOOKUP(B3,EndDeviceReleaseDetails!A$2:H$10000,3,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="E3" t="e">
+        <f>VLOOKUP(B3,EndDeviceReleaseDetails!A$2:H$10000,4,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="F3" t="e">
+        <f>VLOOKUP(B3,EndDeviceReleaseDetails!A$2:H$10000,5,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="G3" t="e">
+        <f>VLOOKUP(B3,EndDeviceReleaseDetails!A$2:H$10000,6,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="H3" t="e">
+        <f>VLOOKUP(B3,EndDeviceReleaseDetails!A$2:H$10000,7,FALSE)</f>
+        <v>#N/A</v>
+      </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
-      <c r="B4" t="s">
-        <v>10</v>
+      <c r="C4" t="e">
+        <f>VLOOKUP(B4,EndDeviceReleaseDetails!A$2:H$10000,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D4" t="e">
+        <f>VLOOKUP(B4,EndDeviceReleaseDetails!A$2:H$10000,3,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="E4" t="e">
+        <f>VLOOKUP(B4,EndDeviceReleaseDetails!A$2:H$10000,4,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="F4" t="e">
+        <f>VLOOKUP(B4,EndDeviceReleaseDetails!A$2:H$10000,5,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="G4" t="e">
+        <f>VLOOKUP(B4,EndDeviceReleaseDetails!A$2:H$10000,6,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="H4" t="e">
+        <f>VLOOKUP(B4,EndDeviceReleaseDetails!A$2:H$10000,7,FALSE)</f>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>11</v>
       </c>
+      <c r="C5" t="e">
+        <f>VLOOKUP(B5,EndDeviceReleaseDetails!A$2:H$10000,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D5" t="e">
+        <f>VLOOKUP(B5,EndDeviceReleaseDetails!A$2:H$10000,3,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="E5" t="e">
+        <f>VLOOKUP(B5,EndDeviceReleaseDetails!A$2:H$10000,4,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="F5" t="e">
+        <f>VLOOKUP(B5,EndDeviceReleaseDetails!A$2:H$10000,5,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="G5" t="e">
+        <f>VLOOKUP(B5,EndDeviceReleaseDetails!A$2:H$10000,6,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="H5" t="e">
+        <f>VLOOKUP(B5,EndDeviceReleaseDetails!A$2:H$10000,7,FALSE)</f>
+        <v>#N/A</v>
+      </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>12</v>
       </c>
+      <c r="C6" t="e">
+        <f>VLOOKUP(B6,EndDeviceReleaseDetails!A$2:H$10000,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D6" t="e">
+        <f>VLOOKUP(B6,EndDeviceReleaseDetails!A$2:H$10000,3,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="E6" t="e">
+        <f>VLOOKUP(B6,EndDeviceReleaseDetails!A$2:H$10000,4,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="F6" t="e">
+        <f>VLOOKUP(B6,EndDeviceReleaseDetails!A$2:H$10000,5,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="G6" t="e">
+        <f>VLOOKUP(B6,EndDeviceReleaseDetails!A$2:H$10000,6,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="H6" t="e">
+        <f>VLOOKUP(B6,EndDeviceReleaseDetails!A$2:H$10000,7,FALSE)</f>
+        <v>#N/A</v>
+      </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>13</v>
       </c>
+      <c r="C7" t="e">
+        <f>VLOOKUP(B7,EndDeviceReleaseDetails!A$2:H$10000,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D7" t="e">
+        <f>VLOOKUP(B7,EndDeviceReleaseDetails!A$2:H$10000,3,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="E7" t="e">
+        <f>VLOOKUP(B7,EndDeviceReleaseDetails!A$2:H$10000,4,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="F7" t="e">
+        <f>VLOOKUP(B7,EndDeviceReleaseDetails!A$2:H$10000,5,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="G7" t="e">
+        <f>VLOOKUP(B7,EndDeviceReleaseDetails!A$2:H$10000,6,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="H7" t="e">
+        <f>VLOOKUP(B7,EndDeviceReleaseDetails!A$2:H$10000,7,FALSE)</f>
+        <v>#N/A</v>
+      </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>14</v>
       </c>
+      <c r="C8" t="e">
+        <f>VLOOKUP(B8,EndDeviceReleaseDetails!A$2:H$10000,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D8" t="e">
+        <f>VLOOKUP(B8,EndDeviceReleaseDetails!A$2:H$10000,3,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="E8" t="e">
+        <f>VLOOKUP(B8,EndDeviceReleaseDetails!A$2:H$10000,4,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="F8" t="e">
+        <f>VLOOKUP(B8,EndDeviceReleaseDetails!A$2:H$10000,5,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="G8" t="e">
+        <f>VLOOKUP(B8,EndDeviceReleaseDetails!A$2:H$10000,6,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="H8" t="e">
+        <f>VLOOKUP(B8,EndDeviceReleaseDetails!A$2:H$10000,7,FALSE)</f>
+        <v>#N/A</v>
+      </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>15</v>
       </c>
+      <c r="C9" t="e">
+        <f>VLOOKUP(B9,EndDeviceReleaseDetails!A$2:H$10000,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D9" t="e">
+        <f>VLOOKUP(B9,EndDeviceReleaseDetails!A$2:H$10000,3,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="E9" t="e">
+        <f>VLOOKUP(B9,EndDeviceReleaseDetails!A$2:H$10000,4,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="F9" t="e">
+        <f>VLOOKUP(B9,EndDeviceReleaseDetails!A$2:H$10000,5,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="G9" t="e">
+        <f>VLOOKUP(B9,EndDeviceReleaseDetails!A$2:H$10000,6,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="H9" t="e">
+        <f>VLOOKUP(B9,EndDeviceReleaseDetails!A$2:H$10000,7,FALSE)</f>
+        <v>#N/A</v>
+      </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>16</v>
       </c>
+      <c r="C10" t="e">
+        <f>VLOOKUP(B10,EndDeviceReleaseDetails!A$2:H$10000,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D10" t="e">
+        <f>VLOOKUP(B10,EndDeviceReleaseDetails!A$2:H$10000,3,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="E10" t="e">
+        <f>VLOOKUP(B10,EndDeviceReleaseDetails!A$2:H$10000,4,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="F10" t="e">
+        <f>VLOOKUP(B10,EndDeviceReleaseDetails!A$2:H$10000,5,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="G10" t="e">
+        <f>VLOOKUP(B10,EndDeviceReleaseDetails!A$2:H$10000,6,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="H10" t="e">
+        <f>VLOOKUP(B10,EndDeviceReleaseDetails!A$2:H$10000,7,FALSE)</f>
+        <v>#N/A</v>
+      </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>17</v>
       </c>
-      <c r="B11" t="s">
-        <v>18</v>
+      <c r="C11" t="e">
+        <f>VLOOKUP(B11,EndDeviceReleaseDetails!A$2:H$10000,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D11" t="e">
+        <f>VLOOKUP(B11,EndDeviceReleaseDetails!A$2:H$10000,3,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="E11" t="e">
+        <f>VLOOKUP(B11,EndDeviceReleaseDetails!A$2:H$10000,4,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="F11" t="e">
+        <f>VLOOKUP(B11,EndDeviceReleaseDetails!A$2:H$10000,5,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="G11" t="e">
+        <f>VLOOKUP(B11,EndDeviceReleaseDetails!A$2:H$10000,6,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="H11" t="e">
+        <f>VLOOKUP(B11,EndDeviceReleaseDetails!A$2:H$10000,7,FALSE)</f>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>19</v>
       </c>
-      <c r="B12" t="s">
-        <v>10</v>
+      <c r="C12" t="e">
+        <f>VLOOKUP(B12,EndDeviceReleaseDetails!A$2:H$10000,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D12" t="e">
+        <f>VLOOKUP(B12,EndDeviceReleaseDetails!A$2:H$10000,3,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="E12" t="e">
+        <f>VLOOKUP(B12,EndDeviceReleaseDetails!A$2:H$10000,4,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="F12" t="e">
+        <f>VLOOKUP(B12,EndDeviceReleaseDetails!A$2:H$10000,5,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="G12" t="e">
+        <f>VLOOKUP(B12,EndDeviceReleaseDetails!A$2:H$10000,6,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="H12" t="e">
+        <f>VLOOKUP(B12,EndDeviceReleaseDetails!A$2:H$10000,7,FALSE)</f>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>20</v>
       </c>
-      <c r="B13" t="s">
-        <v>21</v>
-      </c>
-      <c r="D13" t="s">
-        <v>22</v>
-      </c>
-      <c r="E13">
-        <v>1355</v>
-      </c>
-      <c r="F13">
-        <v>75</v>
-      </c>
-      <c r="H13">
-        <v>5</v>
+      <c r="C13" t="e">
+        <f>VLOOKUP(B13,EndDeviceReleaseDetails!A$2:H$10000,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D13" t="e">
+        <f>VLOOKUP(B13,EndDeviceReleaseDetails!A$2:H$10000,3,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="E13" t="e">
+        <f>VLOOKUP(B13,EndDeviceReleaseDetails!A$2:H$10000,4,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="F13" t="e">
+        <f>VLOOKUP(B13,EndDeviceReleaseDetails!A$2:H$10000,5,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="G13" t="e">
+        <f>VLOOKUP(B13,EndDeviceReleaseDetails!A$2:H$10000,6,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="H13" t="e">
+        <f>VLOOKUP(B13,EndDeviceReleaseDetails!A$2:H$10000,7,FALSE)</f>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>23</v>
       </c>
-      <c r="B14" t="s">
-        <v>21</v>
-      </c>
-      <c r="D14" t="s">
-        <v>22</v>
+      <c r="C14" t="e">
+        <f>VLOOKUP(B14,EndDeviceReleaseDetails!A$2:H$10000,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D14" t="e">
+        <f>VLOOKUP(B14,EndDeviceReleaseDetails!A$2:H$10000,3,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="E14" t="e">
+        <f>VLOOKUP(B14,EndDeviceReleaseDetails!A$2:H$10000,4,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="F14" t="e">
+        <f>VLOOKUP(B14,EndDeviceReleaseDetails!A$2:H$10000,5,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="G14" t="e">
+        <f>VLOOKUP(B14,EndDeviceReleaseDetails!A$2:H$10000,6,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="H14" t="e">
+        <f>VLOOKUP(B14,EndDeviceReleaseDetails!A$2:H$10000,7,FALSE)</f>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>24</v>
       </c>
-      <c r="B15" t="s">
-        <v>18</v>
+      <c r="C15" t="e">
+        <f>VLOOKUP(B15,EndDeviceReleaseDetails!A$2:H$10000,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D15" t="e">
+        <f>VLOOKUP(B15,EndDeviceReleaseDetails!A$2:H$10000,3,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="E15" t="e">
+        <f>VLOOKUP(B15,EndDeviceReleaseDetails!A$2:H$10000,4,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="F15" t="e">
+        <f>VLOOKUP(B15,EndDeviceReleaseDetails!A$2:H$10000,5,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="G15" t="e">
+        <f>VLOOKUP(B15,EndDeviceReleaseDetails!A$2:H$10000,6,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="H15" t="e">
+        <f>VLOOKUP(B15,EndDeviceReleaseDetails!A$2:H$10000,7,FALSE)</f>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>25</v>
       </c>
-      <c r="B16" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C16" t="e">
+        <f>VLOOKUP(B16,EndDeviceReleaseDetails!A$2:H$10000,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D16" t="e">
+        <f>VLOOKUP(B16,EndDeviceReleaseDetails!A$2:H$10000,3,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="E16" t="e">
+        <f>VLOOKUP(B16,EndDeviceReleaseDetails!A$2:H$10000,4,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="F16" t="e">
+        <f>VLOOKUP(B16,EndDeviceReleaseDetails!A$2:H$10000,5,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="G16" t="e">
+        <f>VLOOKUP(B16,EndDeviceReleaseDetails!A$2:H$10000,6,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="H16" t="e">
+        <f>VLOOKUP(B16,EndDeviceReleaseDetails!A$2:H$10000,7,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>26</v>
       </c>
-      <c r="B17" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C17" t="e">
+        <f>VLOOKUP(B17,EndDeviceReleaseDetails!A$2:H$10000,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D17" t="e">
+        <f>VLOOKUP(B17,EndDeviceReleaseDetails!A$2:H$10000,3,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="E17" t="e">
+        <f>VLOOKUP(B17,EndDeviceReleaseDetails!A$2:H$10000,4,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="F17" t="e">
+        <f>VLOOKUP(B17,EndDeviceReleaseDetails!A$2:H$10000,5,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="G17" t="e">
+        <f>VLOOKUP(B17,EndDeviceReleaseDetails!A$2:H$10000,6,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="H17" t="e">
+        <f>VLOOKUP(B17,EndDeviceReleaseDetails!A$2:H$10000,7,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>27</v>
       </c>
-      <c r="B18" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C18" t="e">
+        <f>VLOOKUP(B18,EndDeviceReleaseDetails!A$2:H$10000,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D18" t="e">
+        <f>VLOOKUP(B18,EndDeviceReleaseDetails!A$2:H$10000,3,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="E18" t="e">
+        <f>VLOOKUP(B18,EndDeviceReleaseDetails!A$2:H$10000,4,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="F18" t="e">
+        <f>VLOOKUP(B18,EndDeviceReleaseDetails!A$2:H$10000,5,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="G18" t="e">
+        <f>VLOOKUP(B18,EndDeviceReleaseDetails!A$2:H$10000,6,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="H18" t="e">
+        <f>VLOOKUP(B18,EndDeviceReleaseDetails!A$2:H$10000,7,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C19" t="e">
+        <f>VLOOKUP(B19,EndDeviceReleaseDetails!A$2:H$10000,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D19" t="e">
+        <f>VLOOKUP(B19,EndDeviceReleaseDetails!A$2:H$10000,3,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="E19" t="e">
+        <f>VLOOKUP(B19,EndDeviceReleaseDetails!A$2:H$10000,4,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="F19" t="e">
+        <f>VLOOKUP(B19,EndDeviceReleaseDetails!A$2:H$10000,5,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="G19" t="e">
+        <f>VLOOKUP(B19,EndDeviceReleaseDetails!A$2:H$10000,6,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="H19" t="e">
+        <f>VLOOKUP(B19,EndDeviceReleaseDetails!A$2:H$10000,7,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C20" t="e">
+        <f>VLOOKUP(B20,EndDeviceReleaseDetails!A$2:H$10000,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D20" t="e">
+        <f>VLOOKUP(B20,EndDeviceReleaseDetails!A$2:H$10000,3,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="E20" t="e">
+        <f>VLOOKUP(B20,EndDeviceReleaseDetails!A$2:H$10000,4,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="F20" t="e">
+        <f>VLOOKUP(B20,EndDeviceReleaseDetails!A$2:H$10000,5,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="G20" t="e">
+        <f>VLOOKUP(B20,EndDeviceReleaseDetails!A$2:H$10000,6,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="H20" t="e">
+        <f>VLOOKUP(B20,EndDeviceReleaseDetails!A$2:H$10000,7,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C21" t="e">
+        <f>VLOOKUP(B21,EndDeviceReleaseDetails!A$2:H$10000,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D21" t="e">
+        <f>VLOOKUP(B21,EndDeviceReleaseDetails!A$2:H$10000,3,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="E21" t="e">
+        <f>VLOOKUP(B21,EndDeviceReleaseDetails!A$2:H$10000,4,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="F21" t="e">
+        <f>VLOOKUP(B21,EndDeviceReleaseDetails!A$2:H$10000,5,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="G21" t="e">
+        <f>VLOOKUP(B21,EndDeviceReleaseDetails!A$2:H$10000,6,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="H21" t="e">
+        <f>VLOOKUP(B21,EndDeviceReleaseDetails!A$2:H$10000,7,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C22" t="e">
+        <f>VLOOKUP(B22,EndDeviceReleaseDetails!A$2:H$10000,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D22" t="e">
+        <f>VLOOKUP(B22,EndDeviceReleaseDetails!A$2:H$10000,3,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="E22" t="e">
+        <f>VLOOKUP(B22,EndDeviceReleaseDetails!A$2:H$10000,4,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="F22" t="e">
+        <f>VLOOKUP(B22,EndDeviceReleaseDetails!A$2:H$10000,5,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="G22" t="e">
+        <f>VLOOKUP(B22,EndDeviceReleaseDetails!A$2:H$10000,6,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="H22" t="e">
+        <f>VLOOKUP(B22,EndDeviceReleaseDetails!A$2:H$10000,7,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C23" t="e">
+        <f>VLOOKUP(B23,EndDeviceReleaseDetails!A$2:H$10000,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D23" t="e">
+        <f>VLOOKUP(B23,EndDeviceReleaseDetails!A$2:H$10000,3,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="E23" t="e">
+        <f>VLOOKUP(B23,EndDeviceReleaseDetails!A$2:H$10000,4,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="F23" t="e">
+        <f>VLOOKUP(B23,EndDeviceReleaseDetails!A$2:H$10000,5,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="G23" t="e">
+        <f>VLOOKUP(B23,EndDeviceReleaseDetails!A$2:H$10000,6,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="H23" t="e">
+        <f>VLOOKUP(B23,EndDeviceReleaseDetails!A$2:H$10000,7,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C24" t="e">
+        <f>VLOOKUP(B24,EndDeviceReleaseDetails!A$2:H$10000,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D24" t="e">
+        <f>VLOOKUP(B24,EndDeviceReleaseDetails!A$2:H$10000,3,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="E24" t="e">
+        <f>VLOOKUP(B24,EndDeviceReleaseDetails!A$2:H$10000,4,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="F24" t="e">
+        <f>VLOOKUP(B24,EndDeviceReleaseDetails!A$2:H$10000,5,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="G24" t="e">
+        <f>VLOOKUP(B24,EndDeviceReleaseDetails!A$2:H$10000,6,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="H24" t="e">
+        <f>VLOOKUP(B24,EndDeviceReleaseDetails!A$2:H$10000,7,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C25" t="e">
+        <f>VLOOKUP(B25,EndDeviceReleaseDetails!A$2:H$10000,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D25" t="e">
+        <f>VLOOKUP(B25,EndDeviceReleaseDetails!A$2:H$10000,3,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="E25" t="e">
+        <f>VLOOKUP(B25,EndDeviceReleaseDetails!A$2:H$10000,4,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="F25" t="e">
+        <f>VLOOKUP(B25,EndDeviceReleaseDetails!A$2:H$10000,5,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="G25" t="e">
+        <f>VLOOKUP(B25,EndDeviceReleaseDetails!A$2:H$10000,6,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="H25" t="e">
+        <f>VLOOKUP(B25,EndDeviceReleaseDetails!A$2:H$10000,7,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C26" t="e">
+        <f>VLOOKUP(B26,EndDeviceReleaseDetails!A$2:H$10000,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D26" t="e">
+        <f>VLOOKUP(B26,EndDeviceReleaseDetails!A$2:H$10000,3,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="E26" t="e">
+        <f>VLOOKUP(B26,EndDeviceReleaseDetails!A$2:H$10000,4,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="F26" t="e">
+        <f>VLOOKUP(B26,EndDeviceReleaseDetails!A$2:H$10000,5,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="G26" t="e">
+        <f>VLOOKUP(B26,EndDeviceReleaseDetails!A$2:H$10000,6,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="H26" t="e">
+        <f>VLOOKUP(B26,EndDeviceReleaseDetails!A$2:H$10000,7,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C27" t="e">
+        <f>VLOOKUP(B27,EndDeviceReleaseDetails!A$2:H$10000,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D27" t="e">
+        <f>VLOOKUP(B27,EndDeviceReleaseDetails!A$2:H$10000,3,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="E27" t="e">
+        <f>VLOOKUP(B27,EndDeviceReleaseDetails!A$2:H$10000,4,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="F27" t="e">
+        <f>VLOOKUP(B27,EndDeviceReleaseDetails!A$2:H$10000,5,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="G27" t="e">
+        <f>VLOOKUP(B27,EndDeviceReleaseDetails!A$2:H$10000,6,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="H27" t="e">
+        <f>VLOOKUP(B27,EndDeviceReleaseDetails!A$2:H$10000,7,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C28" t="e">
+        <f>VLOOKUP(B28,EndDeviceReleaseDetails!A$2:H$10000,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D28" t="e">
+        <f>VLOOKUP(B28,EndDeviceReleaseDetails!A$2:H$10000,3,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="E28" t="e">
+        <f>VLOOKUP(B28,EndDeviceReleaseDetails!A$2:H$10000,4,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="F28" t="e">
+        <f>VLOOKUP(B28,EndDeviceReleaseDetails!A$2:H$10000,5,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="G28" t="e">
+        <f>VLOOKUP(B28,EndDeviceReleaseDetails!A$2:H$10000,6,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="H28" t="e">
+        <f>VLOOKUP(B28,EndDeviceReleaseDetails!A$2:H$10000,7,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C29" t="e">
+        <f>VLOOKUP(B29,EndDeviceReleaseDetails!A$2:H$10000,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D29" t="e">
+        <f>VLOOKUP(B29,EndDeviceReleaseDetails!A$2:H$10000,3,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="E29" t="e">
+        <f>VLOOKUP(B29,EndDeviceReleaseDetails!A$2:H$10000,4,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="F29" t="e">
+        <f>VLOOKUP(B29,EndDeviceReleaseDetails!A$2:H$10000,5,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="G29" t="e">
+        <f>VLOOKUP(B29,EndDeviceReleaseDetails!A$2:H$10000,6,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="H29" t="e">
+        <f>VLOOKUP(B29,EndDeviceReleaseDetails!A$2:H$10000,7,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C30" t="e">
+        <f>VLOOKUP(B30,EndDeviceReleaseDetails!A$2:H$10000,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D30" t="e">
+        <f>VLOOKUP(B30,EndDeviceReleaseDetails!A$2:H$10000,3,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="E30" t="e">
+        <f>VLOOKUP(B30,EndDeviceReleaseDetails!A$2:H$10000,4,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="F30" t="e">
+        <f>VLOOKUP(B30,EndDeviceReleaseDetails!A$2:H$10000,5,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="G30" t="e">
+        <f>VLOOKUP(B30,EndDeviceReleaseDetails!A$2:H$10000,6,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="H30" t="e">
+        <f>VLOOKUP(B30,EndDeviceReleaseDetails!A$2:H$10000,7,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C31" t="e">
+        <f>VLOOKUP(B31,EndDeviceReleaseDetails!A$2:H$10000,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D31" t="e">
+        <f>VLOOKUP(B31,EndDeviceReleaseDetails!A$2:H$10000,3,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="E31" t="e">
+        <f>VLOOKUP(B31,EndDeviceReleaseDetails!A$2:H$10000,4,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="F31" t="e">
+        <f>VLOOKUP(B31,EndDeviceReleaseDetails!A$2:H$10000,5,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="G31" t="e">
+        <f>VLOOKUP(B31,EndDeviceReleaseDetails!A$2:H$10000,6,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="H31" t="e">
+        <f>VLOOKUP(B31,EndDeviceReleaseDetails!A$2:H$10000,7,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C32" t="e">
+        <f>VLOOKUP(B32,EndDeviceReleaseDetails!A$2:H$10000,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D32" t="e">
+        <f>VLOOKUP(B32,EndDeviceReleaseDetails!A$2:H$10000,3,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="E32" t="e">
+        <f>VLOOKUP(B32,EndDeviceReleaseDetails!A$2:H$10000,4,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="F32" t="e">
+        <f>VLOOKUP(B32,EndDeviceReleaseDetails!A$2:H$10000,5,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="G32" t="e">
+        <f>VLOOKUP(B32,EndDeviceReleaseDetails!A$2:H$10000,6,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="H32" t="e">
+        <f>VLOOKUP(B32,EndDeviceReleaseDetails!A$2:H$10000,7,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>42</v>
+      </c>
+      <c r="C33" t="e">
+        <f>VLOOKUP(B33,EndDeviceReleaseDetails!A$2:H$10000,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D33" t="e">
+        <f>VLOOKUP(B33,EndDeviceReleaseDetails!A$2:H$10000,3,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="E33" t="e">
+        <f>VLOOKUP(B33,EndDeviceReleaseDetails!A$2:H$10000,4,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="F33" t="e">
+        <f>VLOOKUP(B33,EndDeviceReleaseDetails!A$2:H$10000,5,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="G33" t="e">
+        <f>VLOOKUP(B33,EndDeviceReleaseDetails!A$2:H$10000,6,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="H33" t="e">
+        <f>VLOOKUP(B33,EndDeviceReleaseDetails!A$2:H$10000,7,FALSE)</f>
+        <v>#N/A</v>
       </c>
     </row>
   </sheetData>
@@ -1208,16 +1949,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="36.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -1243,6 +1989,71 @@
         <v>6</v>
       </c>
     </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2">
+        <v>1355</v>
+      </c>
+      <c r="E2">
+        <v>75</v>
+      </c>
+      <c r="G2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3">
+        <v>1342</v>
+      </c>
+      <c r="E3">
+        <v>75</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4">
+        <v>1342</v>
+      </c>
+      <c r="E4">
+        <v>65</v>
+      </c>
+      <c r="G4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C13" t="s">
+        <v>22</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>